<commit_message>
Correccion de errores ortograficos del documento.
</commit_message>
<xml_diff>
--- a/repository/S.A.P.O/Producto/Iteraciones/Iteracion_01/02_Documento_Requerimiento/Funcionalidad por Paquetes.xlsx
+++ b/repository/S.A.P.O/Producto/Iteraciones/Iteracion_01/02_Documento_Requerimiento/Funcionalidad por Paquetes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Funcionalidad por Paquete" sheetId="1" r:id="rId1"/>
@@ -16,23 +16,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="191">
   <si>
     <t>Paquete</t>
   </si>
   <si>
-    <t>Nro CU</t>
-  </si>
-  <si>
     <t>Casos de Uso</t>
   </si>
   <si>
     <t>Objetivo</t>
   </si>
   <si>
-    <t>Administracion de Sistema</t>
-  </si>
-  <si>
     <t>Registrar usuario</t>
   </si>
   <si>
@@ -81,18 +75,9 @@
     <t>Dar de baja a un rol</t>
   </si>
   <si>
-    <t>Registrar asignacion de rol</t>
-  </si>
-  <si>
     <t>Registra a un usuario uno o varios roles</t>
   </si>
   <si>
-    <t>Eliminar asignacion de rol</t>
-  </si>
-  <si>
-    <t>Elimina una asignacion de rol de un usuario</t>
-  </si>
-  <si>
     <t>Registrar permiso de usuario</t>
   </si>
   <si>
@@ -138,12 +123,6 @@
     <t>Consultar estado</t>
   </si>
   <si>
-    <t>Cinsultar un estado del sistema</t>
-  </si>
-  <si>
-    <t>Administracio de sesion de usuario</t>
-  </si>
-  <si>
     <t>Iniciar sesión</t>
   </si>
   <si>
@@ -174,54 +153,6 @@
     <t>Recuperar la Password de un usuario del sistema</t>
   </si>
   <si>
-    <t>Gestion de Historias Clinicas</t>
-  </si>
-  <si>
-    <t>Registrar Historia Clinica</t>
-  </si>
-  <si>
-    <t>Registrar los datos de una Historia Clinica en el sistema</t>
-  </si>
-  <si>
-    <t>Modificar Historia Clinica</t>
-  </si>
-  <si>
-    <t>Modificar los datos de una Historia Clinica en el sistema</t>
-  </si>
-  <si>
-    <t>Consultar Historia Clinica</t>
-  </si>
-  <si>
-    <t>Consulta los datos de cada atencion realizada a cada paciente segun diferentes criterios de consulta</t>
-  </si>
-  <si>
-    <t>Imprimir Historia Clinica</t>
-  </si>
-  <si>
-    <t>Imprime una Historia Clinica</t>
-  </si>
-  <si>
-    <t>Registrar Atencion en Historia Clinica</t>
-  </si>
-  <si>
-    <t>Registrar los datos de una atencion en una Historia Clinica en el sistema</t>
-  </si>
-  <si>
-    <t>Modificar Atencion en Historia Clinica</t>
-  </si>
-  <si>
-    <t>Modificar los datos de una atencion en una Historia Clinica en el sistema</t>
-  </si>
-  <si>
-    <t>Eliminar Atencion en Historia Clinica</t>
-  </si>
-  <si>
-    <t>Eliminar los datos de una atencion en una Historia Clinica en el sistema</t>
-  </si>
-  <si>
-    <t>Gestion de Pacientes</t>
-  </si>
-  <si>
     <t>Registrar Paciente</t>
   </si>
   <si>
@@ -240,30 +171,12 @@
     <t>Visualizar los datos de un Paciente en el sistema</t>
   </si>
   <si>
-    <t>Asignar Historia Clinica al Paciente</t>
-  </si>
-  <si>
     <t>Buscar Paciente</t>
   </si>
   <si>
-    <t>Buscar pacientes en funcion de criterios predefinidos</t>
-  </si>
-  <si>
-    <t>Gestion de Informes</t>
-  </si>
-  <si>
     <t>Generar Informes de atenciones</t>
   </si>
   <si>
-    <t>Genera informe de atenciones en un periodo de tiempo, en funcion de criterios predefinidos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generar Informes de sintomas </t>
-  </si>
-  <si>
-    <t>Genera informe de sintomas en un periodo de tiempo, en funcion de criterios predefinidos</t>
-  </si>
-  <si>
     <t>Gestion de Profesores</t>
   </si>
   <si>
@@ -330,30 +243,6 @@
     <t>Registrar los tipos de atención que se pueden realizar en cada cátedra.</t>
   </si>
   <si>
-    <t>Registrar horarios de catedra</t>
-  </si>
-  <si>
-    <t>Registra los horarios de cada una de las catedras en el sistema</t>
-  </si>
-  <si>
-    <t>Modificar horarios de catedra</t>
-  </si>
-  <si>
-    <t>Modifica los horarios de cada una de las catedras en el sistema</t>
-  </si>
-  <si>
-    <t>Eliminar horarios de catedra</t>
-  </si>
-  <si>
-    <t>Elimina los horarios de cada una de las catedras del sistema</t>
-  </si>
-  <si>
-    <t>Consultar horarios de catedra</t>
-  </si>
-  <si>
-    <t>Consultar los horarios de cada una de las catedras del sistema</t>
-  </si>
-  <si>
     <t>Gestión de Alumnos</t>
   </si>
   <si>
@@ -381,45 +270,6 @@
     <t>Eliminar un alumno registrado.</t>
   </si>
   <si>
-    <t>Registrar derivacion de paciente</t>
-  </si>
-  <si>
-    <t>Registrar la derivacion de un paciente hacia una catedra</t>
-  </si>
-  <si>
-    <t>Eliminar derivacion</t>
-  </si>
-  <si>
-    <t>Elimina la derivacion de un paciente a una catedra</t>
-  </si>
-  <si>
-    <t>Modificar derivacion</t>
-  </si>
-  <si>
-    <t>Actualiza la derivacion de un paciente a una catedra</t>
-  </si>
-  <si>
-    <t>Administracion de Asignaciones</t>
-  </si>
-  <si>
-    <t>Registrar asignacion de paciente</t>
-  </si>
-  <si>
-    <t>Registrar la asignacion de un paciente a un alumno</t>
-  </si>
-  <si>
-    <t>Modificar asignacion de paciente</t>
-  </si>
-  <si>
-    <t>Modificar asignacion de paciente a alumno</t>
-  </si>
-  <si>
-    <t>Eliminar asignacion de paciente</t>
-  </si>
-  <si>
-    <t>Eliminar asignacion de paciente a alumno</t>
-  </si>
-  <si>
     <t>Consultar asignaciones</t>
   </si>
   <si>
@@ -585,13 +435,160 @@
     <t>La SeCyT pretende que el sistema tienda a minimizar el uso del papel mediante la generación y uso de la mayor cantidad de archivos y documentos electrónicos e imágenes digitales. También solicitó que los documentos presentados al momento de presentar la Solicitud de Inscripción  del Centro de Investigación sean digitalizados mediante algún dispositivo.</t>
   </si>
   <si>
-    <t>Administracion de Derivaciones</t>
-  </si>
-  <si>
-    <t>Confirmar asignacion por parte de un alumno</t>
-  </si>
-  <si>
     <t>Autoridad</t>
+  </si>
+  <si>
+    <t>Registrar horarios de cátedra</t>
+  </si>
+  <si>
+    <t>Registra los horarios de cada una de las cátedras en el sistema</t>
+  </si>
+  <si>
+    <t>Modificar horarios de cátedra</t>
+  </si>
+  <si>
+    <t>Modifica los horarios de cada una de las cátedras en el sistema</t>
+  </si>
+  <si>
+    <t>Eliminar horarios de cátedra</t>
+  </si>
+  <si>
+    <t>Elimina los horarios de cada una de las cátedras del sistema</t>
+  </si>
+  <si>
+    <t>Consultar horarios de cátedra</t>
+  </si>
+  <si>
+    <t>Consultar los horarios de cada una de las cátedras del sistema</t>
+  </si>
+  <si>
+    <t>Administración de Derivaciones</t>
+  </si>
+  <si>
+    <t>Registrar derivación de paciente</t>
+  </si>
+  <si>
+    <t>Registrar la derivación de un paciente hacia una cátedra</t>
+  </si>
+  <si>
+    <t>Eliminar derivación</t>
+  </si>
+  <si>
+    <t>Elimina la derivación de un paciente a una cátedra</t>
+  </si>
+  <si>
+    <t>Modificar derivación</t>
+  </si>
+  <si>
+    <t>Actualiza la derivación de un paciente a una cátedra</t>
+  </si>
+  <si>
+    <t>Administración de Asignaciones</t>
+  </si>
+  <si>
+    <t>Registrar asignación de paciente</t>
+  </si>
+  <si>
+    <t>Registrar la asignación de un paciente a un alumno</t>
+  </si>
+  <si>
+    <t>Modificar asignación de paciente</t>
+  </si>
+  <si>
+    <t>Modificar asignación de paciente a alumno</t>
+  </si>
+  <si>
+    <t>Eliminar asignación de paciente</t>
+  </si>
+  <si>
+    <t>Eliminar asignación de paciente a alumno</t>
+  </si>
+  <si>
+    <t>Confirmar asignación por parte de un alumno</t>
+  </si>
+  <si>
+    <t>Nro. CU</t>
+  </si>
+  <si>
+    <t>Administración de Sistema</t>
+  </si>
+  <si>
+    <t>Registrar asignación de rol</t>
+  </si>
+  <si>
+    <t>Eliminar asignación de rol</t>
+  </si>
+  <si>
+    <t>Elimina una asignación de rol de un usuario</t>
+  </si>
+  <si>
+    <t>Consultar un estado del sistema</t>
+  </si>
+  <si>
+    <t>Administración de sesión de usuario</t>
+  </si>
+  <si>
+    <t>Gestión de Historias Clínicas</t>
+  </si>
+  <si>
+    <t>Registrar Historia Clínica</t>
+  </si>
+  <si>
+    <t>Registrar los datos de una Historia Clínica en el sistema</t>
+  </si>
+  <si>
+    <t>Modificar Historia Clínica</t>
+  </si>
+  <si>
+    <t>Modificar los datos de una Historia Clínica en el sistema</t>
+  </si>
+  <si>
+    <t>Consultar Historia Clínica</t>
+  </si>
+  <si>
+    <t>Consulta los datos de cada atención realizada a cada paciente según diferentes criterios de consulta</t>
+  </si>
+  <si>
+    <t>Imprimir Historia Clínica</t>
+  </si>
+  <si>
+    <t>Imprime una Historia Clínica</t>
+  </si>
+  <si>
+    <t>Registrar Atención en Historia Clínica</t>
+  </si>
+  <si>
+    <t>Registrar los datos de una atención en una Historia Clínica en el sistema</t>
+  </si>
+  <si>
+    <t>Modificar Atención en Historia Clínica</t>
+  </si>
+  <si>
+    <t>Modificar los datos de una atención en una Historia Clínica en el sistema</t>
+  </si>
+  <si>
+    <t>Eliminar Atención en Historia Clínica</t>
+  </si>
+  <si>
+    <t>Eliminar los datos de una atención en una Historia Clínica en el sistema</t>
+  </si>
+  <si>
+    <t>Gestión de Pacientes</t>
+  </si>
+  <si>
+    <t>Buscar pacientes en función de criterios predefinidos</t>
+  </si>
+  <si>
+    <t>Gestión de Informes</t>
+  </si>
+  <si>
+    <t>Genera informe de atenciones en un periodo de tiempo, en función de criterios predefinidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generar Informes de síntomas </t>
+  </si>
+  <si>
+    <t>Genera informe de síntomas en un periodo de tiempo, en función de criterios predefinidos</t>
   </si>
 </sst>
 </file>
@@ -721,6 +718,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -728,9 +728,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1027,10 +1024,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1046,794 +1043,784 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="11" t="s">
-        <v>4</v>
+      <c r="A2" s="12" t="s">
+        <v>164</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="12"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="4">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="12"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="4">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="12"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="4">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="12"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="4">
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="12"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="4">
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="12"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="4">
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="12"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="4">
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="12"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="4">
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>21</v>
+        <v>165</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="12"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="4">
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>24</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30">
-      <c r="A12" s="12"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="4">
         <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="12"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="4">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="12"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="4">
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="12"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="4">
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="12"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="4">
         <v>15</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="12"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="4">
         <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="12"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="4">
         <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="13"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="4">
         <v>18</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>40</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30">
-      <c r="A20" s="11" t="s">
-        <v>41</v>
+      <c r="A20" s="12" t="s">
+        <v>169</v>
       </c>
       <c r="B20" s="4">
         <v>19</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30">
-      <c r="A21" s="12"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="4">
         <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30">
-      <c r="A22" s="12"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="4">
         <v>21</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="30">
-      <c r="A23" s="12"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="4">
         <v>22</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30">
-      <c r="A24" s="13"/>
+      <c r="A24" s="14"/>
       <c r="B24" s="4">
         <v>23</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30">
-      <c r="A25" s="11" t="s">
-        <v>52</v>
+      <c r="A25" s="12" t="s">
+        <v>170</v>
       </c>
       <c r="B25" s="4">
         <v>24</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>53</v>
+        <v>171</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>54</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30">
-      <c r="A26" s="12"/>
+      <c r="A26" s="13"/>
       <c r="B26" s="4">
         <v>25</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>55</v>
+        <v>173</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>56</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="45">
-      <c r="A27" s="12"/>
+      <c r="A27" s="13"/>
       <c r="B27" s="4">
         <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>57</v>
+        <v>175</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>58</v>
+        <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="12"/>
+      <c r="A28" s="13"/>
       <c r="B28" s="4">
         <v>27</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>59</v>
+        <v>177</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>60</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30">
-      <c r="A29" s="12"/>
+      <c r="A29" s="13"/>
       <c r="B29" s="4">
         <v>28</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>61</v>
+        <v>179</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>62</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="30">
-      <c r="A30" s="12"/>
+      <c r="A30" s="13"/>
       <c r="B30" s="4">
         <v>29</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>63</v>
+        <v>181</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>64</v>
+        <v>182</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="30">
-      <c r="A31" s="13"/>
+      <c r="A31" s="14"/>
       <c r="B31" s="4">
         <v>30</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>65</v>
+        <v>183</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>66</v>
+        <v>184</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30">
-      <c r="A32" s="11" t="s">
-        <v>67</v>
+      <c r="A32" s="12" t="s">
+        <v>185</v>
       </c>
       <c r="B32" s="4">
         <v>31</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="30">
-      <c r="A33" s="12"/>
+      <c r="A33" s="13"/>
       <c r="B33" s="4">
         <v>32</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="30">
-      <c r="A34" s="12"/>
+      <c r="A34" s="13"/>
       <c r="B34" s="4">
         <v>33</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="12"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="30">
+      <c r="A35" s="14"/>
       <c r="B35" s="4">
         <v>34</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="1:4" ht="30">
-      <c r="A36" s="13"/>
+        <v>51</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="45">
+      <c r="A36" s="12" t="s">
+        <v>187</v>
+      </c>
       <c r="B36" s="4">
         <v>35</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="45">
-      <c r="A37" s="11" t="s">
-        <v>77</v>
-      </c>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="30">
+      <c r="A37" s="14"/>
       <c r="B37" s="4">
         <v>36</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>78</v>
+        <v>189</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="30">
-      <c r="A38" s="13"/>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="B38" s="4">
         <v>37</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="11" t="s">
-        <v>82</v>
-      </c>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="30">
+      <c r="A39" s="13"/>
       <c r="B39" s="4">
         <v>38</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="30">
-      <c r="A40" s="12"/>
+      <c r="A40" s="14"/>
       <c r="B40" s="4">
         <v>39</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="30">
-      <c r="A41" s="13"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="12" t="s">
+        <v>60</v>
+      </c>
       <c r="B41" s="4">
         <v>40</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="11" t="s">
-        <v>89</v>
-      </c>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="30">
+      <c r="A42" s="13"/>
       <c r="B42" s="4">
         <v>41</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="30">
-      <c r="A43" s="12"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="13"/>
       <c r="B43" s="4">
         <v>42</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>92</v>
+        <v>65</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="12"/>
+      <c r="A44" s="13"/>
       <c r="B44" s="4">
         <v>43</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="12"/>
+      <c r="A45" s="13"/>
       <c r="B45" s="4">
         <v>44</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>96</v>
+        <v>69</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>97</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="12"/>
+      <c r="A46" s="13"/>
       <c r="B46" s="4">
         <v>45</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="12"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="30">
+      <c r="A47" s="13"/>
       <c r="B47" s="4">
         <v>46</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>100</v>
+        <v>73</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="30">
-      <c r="A48" s="12"/>
+      <c r="A48" s="13"/>
       <c r="B48" s="4">
         <v>47</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>102</v>
+        <v>140</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>103</v>
+        <v>141</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="30">
-      <c r="A49" s="12"/>
+      <c r="A49" s="13"/>
       <c r="B49" s="4">
         <v>48</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>104</v>
+        <v>142</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>105</v>
+        <v>143</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="30">
-      <c r="A50" s="12"/>
+      <c r="A50" s="13"/>
       <c r="B50" s="4">
         <v>49</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>106</v>
+        <v>144</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>107</v>
+        <v>145</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="30">
-      <c r="A51" s="12"/>
+      <c r="A51" s="14"/>
       <c r="B51" s="4">
         <v>50</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>108</v>
+        <v>146</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="30">
-      <c r="A52" s="13"/>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="12" t="s">
+        <v>75</v>
+      </c>
       <c r="B52" s="4">
         <v>51</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>111</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="11" t="s">
-        <v>112</v>
-      </c>
+      <c r="A53" s="13"/>
       <c r="B53" s="4">
         <v>52</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="12"/>
+      <c r="A54" s="13"/>
       <c r="B54" s="4">
         <v>53</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="12"/>
+      <c r="A55" s="14"/>
       <c r="B55" s="4">
         <v>54</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="13"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="30">
+      <c r="A56" s="12" t="s">
+        <v>148</v>
+      </c>
       <c r="B56" s="4">
         <v>55</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>119</v>
+        <v>149</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>120</v>
+        <v>150</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="30">
-      <c r="A57" s="11" t="s">
-        <v>189</v>
-      </c>
+      <c r="A57" s="13"/>
       <c r="B57" s="4">
         <v>56</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>121</v>
+        <v>151</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>122</v>
+        <v>152</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="30">
-      <c r="A58" s="12"/>
+      <c r="A58" s="14"/>
       <c r="B58" s="4">
         <v>57</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>124</v>
+        <v>154</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="30">
-      <c r="A59" s="13"/>
+      <c r="A59" s="12" t="s">
+        <v>155</v>
+      </c>
       <c r="B59" s="4">
         <v>58</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>125</v>
+        <v>156</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="30">
-      <c r="A60" s="11" t="s">
-        <v>127</v>
-      </c>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="13"/>
       <c r="B60" s="4">
         <v>59</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>128</v>
+        <v>158</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>129</v>
+        <v>159</v>
       </c>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="12"/>
+      <c r="A61" s="13"/>
       <c r="B61" s="4">
         <v>60</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>131</v>
+        <v>161</v>
       </c>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="12"/>
+      <c r="A62" s="14"/>
       <c r="B62" s="4">
         <v>61</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>132</v>
+        <v>84</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="13"/>
-      <c r="B63" s="4">
-        <v>62</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="30">
-      <c r="C64" s="1" t="s">
-        <v>190</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="30">
+      <c r="C63" s="1" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A42:A52"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A41:A51"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="A59:A62"/>
     <mergeCell ref="A2:A19"/>
     <mergeCell ref="A20:A24"/>
     <mergeCell ref="A25:A31"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -1845,7 +1832,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1856,67 +1843,67 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>137</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30">
       <c r="A2" s="5" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>139</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="60">
       <c r="A3" s="5" t="s">
-        <v>140</v>
+        <v>90</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>141</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30">
       <c r="A4" s="5" t="s">
-        <v>142</v>
+        <v>92</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>143</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30">
       <c r="A5" s="5" t="s">
-        <v>144</v>
+        <v>94</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>145</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="45">
       <c r="A6" s="5" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>147</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="5" t="s">
-        <v>148</v>
+        <v>98</v>
       </c>
       <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="5" t="s">
-        <v>149</v>
+        <v>99</v>
       </c>
       <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="14" t="s">
-        <v>191</v>
+      <c r="A9" s="11" t="s">
+        <v>139</v>
       </c>
       <c r="B9" s="3"/>
     </row>
@@ -1930,7 +1917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -1943,145 +1930,145 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>151</v>
+        <v>101</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>152</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="45">
       <c r="A2" s="5" t="s">
-        <v>153</v>
+        <v>103</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>154</v>
+        <v>104</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>155</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30">
       <c r="A3" s="5" t="s">
-        <v>156</v>
+        <v>106</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>157</v>
+        <v>107</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>158</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="60">
       <c r="A4" s="5" t="s">
-        <v>159</v>
+        <v>109</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>161</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="75">
       <c r="A5" s="5" t="s">
-        <v>162</v>
+        <v>112</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>164</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="60">
       <c r="A6" s="5" t="s">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>166</v>
+        <v>116</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>167</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="60">
       <c r="A7" s="5" t="s">
-        <v>168</v>
+        <v>118</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>169</v>
+        <v>119</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>170</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="45">
       <c r="A8" s="5" t="s">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>172</v>
+        <v>122</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>173</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="60">
       <c r="A9" s="5" t="s">
-        <v>174</v>
+        <v>124</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>175</v>
+        <v>125</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>176</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="60">
       <c r="A10" s="5" t="s">
-        <v>177</v>
+        <v>127</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>178</v>
+        <v>128</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="5" t="s">
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>181</v>
+        <v>131</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="60">
       <c r="A12" s="5" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>184</v>
+        <v>134</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>185</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="105">
       <c r="A13" s="5" t="s">
-        <v>186</v>
+        <v>136</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>187</v>
+        <v>137</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>188</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Eliminado caso de uso de registrar confirmacion de asignacion de pacientes.
</commit_message>
<xml_diff>
--- a/repository/S.A.P.O/Producto/Iteraciones/Iteracion_01/02_Documento_Requerimiento/Funcionalidad por Paquetes.xlsx
+++ b/repository/S.A.P.O/Producto/Iteraciones/Iteracion_01/02_Documento_Requerimiento/Funcionalidad por Paquetes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="190">
   <si>
     <t>Paquete</t>
   </si>
@@ -502,9 +502,6 @@
   </si>
   <si>
     <t>Eliminar asignación de paciente a alumno</t>
-  </si>
-  <si>
-    <t>Confirmar asignación por parte de un alumno</t>
   </si>
   <si>
     <t>Nro. CU</t>
@@ -1026,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1043,7 +1040,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>1</v>
@@ -1054,7 +1051,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -1156,7 +1153,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>19</v>
@@ -1168,10 +1165,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30">
@@ -1267,12 +1264,12 @@
         <v>34</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30">
       <c r="A20" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B20" s="4">
         <v>19</v>
@@ -1334,16 +1331,16 @@
     </row>
     <row r="25" spans="1:4" ht="30">
       <c r="A25" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B25" s="4">
         <v>24</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30">
@@ -1352,10 +1349,10 @@
         <v>25</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="45">
@@ -1364,10 +1361,10 @@
         <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1376,10 +1373,10 @@
         <v>27</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30">
@@ -1388,10 +1385,10 @@
         <v>28</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="30">
@@ -1400,10 +1397,10 @@
         <v>29</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="30">
@@ -1412,15 +1409,15 @@
         <v>30</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30">
       <c r="A32" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B32" s="4">
         <v>31</v>
@@ -1465,12 +1462,12 @@
         <v>51</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="45">
       <c r="A36" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B36" s="4">
         <v>35</v>
@@ -1479,7 +1476,7 @@
         <v>52</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="30">
@@ -1488,10 +1485,10 @@
         <v>36</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1804,10 +1801,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="30">
-      <c r="C63" s="1" t="s">
-        <v>162</v>
-      </c>
+    <row r="63" spans="1:4">
+      <c r="C63" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
Se agrego la descripcion del Responsable de Recepcion de Pacientes
</commit_message>
<xml_diff>
--- a/repository/S.A.P.O/Producto/Iteraciones/Iteracion_01/02_Documento_Requerimiento/Funcionalidad por Paquetes.xlsx
+++ b/repository/S.A.P.O/Producto/Iteraciones/Iteracion_01/02_Documento_Requerimiento/Funcionalidad por Paquetes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Funcionalidad por Paquete" sheetId="1" r:id="rId1"/>
@@ -156,21 +156,12 @@
     <t>Registrar Paciente</t>
   </si>
   <si>
-    <t>Registrar los datos de un Paciente en el sistema</t>
-  </si>
-  <si>
     <t>Modificar Paciente</t>
   </si>
   <si>
-    <t>Modificar los datos de un Paciente en el sistema</t>
-  </si>
-  <si>
     <t>Consultar Paciente</t>
   </si>
   <si>
-    <t>Visualizar los datos de un Paciente en el sistema</t>
-  </si>
-  <si>
     <t>Buscar Paciente</t>
   </si>
   <si>
@@ -297,9 +288,6 @@
     <t>Reloj</t>
   </si>
   <si>
-    <t>Realiza  las anulaciones de asignaciones. (completar).</t>
-  </si>
-  <si>
     <t>Alumno</t>
   </si>
   <si>
@@ -525,15 +513,6 @@
     <t>Administración de sesión de usuario</t>
   </si>
   <si>
-    <t>Gestión de Historias Clínicas</t>
-  </si>
-  <si>
-    <t>Registrar Historia Clínica</t>
-  </si>
-  <si>
-    <t>Registrar los datos de una Historia Clínica en el sistema</t>
-  </si>
-  <si>
     <t>Modificar Historia Clínica</t>
   </si>
   <si>
@@ -570,9 +549,6 @@
     <t>Eliminar los datos de una atención en una Historia Clínica en el sistema</t>
   </si>
   <si>
-    <t>Gestión de Pacientes</t>
-  </si>
-  <si>
     <t>Buscar pacientes en función de criterios predefinidos</t>
   </si>
   <si>
@@ -586,6 +562,30 @@
   </si>
   <si>
     <t>Genera informe de síntomas en un periodo de tiempo, en función de criterios predefinidos</t>
+  </si>
+  <si>
+    <t>Gestión de Historias Clínicas y Pacientes</t>
+  </si>
+  <si>
+    <t>Registrar los datos basicos de un Paciente en el sistema</t>
+  </si>
+  <si>
+    <t>Modificar los datos basicos de un Paciente en el sistema</t>
+  </si>
+  <si>
+    <t>Visualizar los datos basicos de un Paciente en el sistema</t>
+  </si>
+  <si>
+    <t>Generar Historia Clínica</t>
+  </si>
+  <si>
+    <t>Generar una Historia Clínica vacía en el sistema para un paciente</t>
+  </si>
+  <si>
+    <t>Responsable de cargar los datos básicos de un paciente cuando se presenta en Recepción para ser atendido.</t>
+  </si>
+  <si>
+    <t>Se encarga de realizar las tareas automáticas del sistema, como anulaciones o generacion de Historias Clinicas.</t>
   </si>
 </sst>
 </file>
@@ -685,7 +685,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -727,6 +727,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1023,13 +1027,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.5703125" style="1" customWidth="1"/>
@@ -1040,7 +1044,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>1</v>
@@ -1051,7 +1055,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="12" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -1153,7 +1157,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>19</v>
@@ -1165,10 +1169,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30">
@@ -1264,12 +1268,12 @@
         <v>34</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30">
       <c r="A20" s="12" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B20" s="4">
         <v>19</v>
@@ -1331,16 +1335,16 @@
     </row>
     <row r="25" spans="1:4" ht="30">
       <c r="A25" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="B25" s="4">
+        <v>182</v>
+      </c>
+      <c r="B25" s="15">
         <v>24</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>171</v>
+      <c r="C25" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30">
@@ -1349,10 +1353,10 @@
         <v>25</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="45">
@@ -1361,10 +1365,10 @@
         <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1373,10 +1377,10 @@
         <v>27</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30">
@@ -1385,10 +1389,10 @@
         <v>28</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="30">
@@ -1397,28 +1401,26 @@
         <v>29</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="30">
-      <c r="A31" s="14"/>
+      <c r="A31" s="13"/>
       <c r="B31" s="4">
         <v>30</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30">
-      <c r="A32" s="12" t="s">
-        <v>184</v>
-      </c>
+      <c r="A32" s="13"/>
       <c r="B32" s="4">
         <v>31</v>
       </c>
@@ -1426,7 +1428,7 @@
         <v>45</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>46</v>
+        <v>183</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="30">
@@ -1435,10 +1437,10 @@
         <v>32</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>48</v>
+        <v>184</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="30">
@@ -1447,10 +1449,10 @@
         <v>33</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>50</v>
+        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30">
@@ -1459,24 +1461,24 @@
         <v>34</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="45">
       <c r="A36" s="12" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B36" s="4">
         <v>35</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="30">
@@ -1485,24 +1487,24 @@
         <v>36</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B38" s="4">
         <v>37</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="30">
@@ -1511,10 +1513,10 @@
         <v>38</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="30">
@@ -1523,24 +1525,24 @@
         <v>39</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B41" s="4">
         <v>40</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="30">
@@ -1549,10 +1551,10 @@
         <v>41</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1561,10 +1563,10 @@
         <v>42</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1573,10 +1575,10 @@
         <v>43</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1585,10 +1587,10 @@
         <v>44</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1597,10 +1599,10 @@
         <v>45</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="30">
@@ -1609,10 +1611,10 @@
         <v>46</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="30">
@@ -1621,10 +1623,10 @@
         <v>47</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="30">
@@ -1633,10 +1635,10 @@
         <v>48</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="30">
@@ -1645,10 +1647,10 @@
         <v>49</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="30">
@@ -1657,24 +1659,24 @@
         <v>50</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B52" s="4">
         <v>51</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1683,10 +1685,10 @@
         <v>52</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1695,10 +1697,10 @@
         <v>53</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1707,24 +1709,24 @@
         <v>54</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="30">
       <c r="A56" s="12" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B56" s="4">
         <v>55</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="30">
@@ -1733,10 +1735,10 @@
         <v>56</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="30">
@@ -1745,24 +1747,24 @@
         <v>57</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="30">
       <c r="A59" s="12" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B59" s="4">
         <v>58</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1771,10 +1773,10 @@
         <v>59</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1783,10 +1785,10 @@
         <v>60</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1795,27 +1797,26 @@
         <v>61</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="C63" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="A41:A51"/>
     <mergeCell ref="A52:A55"/>
     <mergeCell ref="A56:A58"/>
     <mergeCell ref="A59:A62"/>
     <mergeCell ref="A2:A19"/>
     <mergeCell ref="A20:A24"/>
-    <mergeCell ref="A25:A31"/>
-    <mergeCell ref="A32:A35"/>
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A25:A35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -1826,8 +1827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1838,67 +1839,69 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30">
       <c r="A2" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="60">
       <c r="A3" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="30">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="45">
       <c r="A4" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>93</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30">
       <c r="A5" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="45">
       <c r="A6" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="45">
       <c r="A8" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B8" s="3"/>
+        <v>95</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B9" s="3"/>
     </row>
@@ -1925,145 +1928,145 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="45">
       <c r="A2" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30">
       <c r="A3" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="60">
       <c r="A4" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="75">
       <c r="A5" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="60">
       <c r="A6" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="60">
       <c r="A7" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="45">
       <c r="A8" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="60">
       <c r="A9" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="60">
       <c r="A10" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="60">
       <c r="A12" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="105">
       <c r="A13" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se modificar algunos nombres y objetivos de los casos de uso buscar y consultar
</commit_message>
<xml_diff>
--- a/repository/S.A.P.O/Producto/Iteraciones/Iteracion_01/02_Documento_Requerimiento/Funcionalidad por Paquetes.xlsx
+++ b/repository/S.A.P.O/Producto/Iteraciones/Iteracion_01/02_Documento_Requerimiento/Funcionalidad por Paquetes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="192">
   <si>
     <t>Paquete</t>
   </si>
@@ -243,12 +243,6 @@
     <t>Registrar los datos de un nuevo alumno.</t>
   </si>
   <si>
-    <t>Consultar alumno</t>
-  </si>
-  <si>
-    <t>Visualizar los datos de un alumno registrado.</t>
-  </si>
-  <si>
     <t>Modificar alumno</t>
   </si>
   <si>
@@ -543,15 +537,6 @@
     <t>Modificar los datos de una atención en una Historia Clínica en el sistema</t>
   </si>
   <si>
-    <t>Eliminar Atención en Historia Clínica</t>
-  </si>
-  <si>
-    <t>Eliminar los datos de una atención en una Historia Clínica en el sistema</t>
-  </si>
-  <si>
-    <t>Buscar pacientes en función de criterios predefinidos</t>
-  </si>
-  <si>
     <t>Gestión de Informes</t>
   </si>
   <si>
@@ -567,25 +552,46 @@
     <t>Gestión de Historias Clínicas y Pacientes</t>
   </si>
   <si>
-    <t>Registrar los datos basicos de un Paciente en el sistema</t>
-  </si>
-  <si>
     <t>Modificar los datos basicos de un Paciente en el sistema</t>
   </si>
   <si>
-    <t>Visualizar los datos basicos de un Paciente en el sistema</t>
-  </si>
-  <si>
-    <t>Generar Historia Clínica</t>
-  </si>
-  <si>
-    <t>Generar una Historia Clínica vacía en el sistema para un paciente</t>
-  </si>
-  <si>
     <t>Responsable de cargar los datos básicos de un paciente cuando se presenta en Recepción para ser atendido.</t>
   </si>
   <si>
     <t>Se encarga de realizar las tareas automáticas del sistema, como anulaciones o generacion de Historias Clinicas.</t>
+  </si>
+  <si>
+    <t>Verificar la existencia de un paciente en el sistema.</t>
+  </si>
+  <si>
+    <t>Buscar pacientes registrados en el sistema en función de ciertos parámetros</t>
+  </si>
+  <si>
+    <t>Asignar Paciente</t>
+  </si>
+  <si>
+    <t>Asignacion de un paciente para si mismo por parte del alumno</t>
+  </si>
+  <si>
+    <t>Registrar Diagnostico</t>
+  </si>
+  <si>
+    <t>Registrar en el sistema los distintos problemas del paciente que seran objeto de atenciones .</t>
+  </si>
+  <si>
+    <t>Registrar los datos basicos de un Paciente en el sistema generando su correspondiente Historia Clinica.</t>
+  </si>
+  <si>
+    <t>Donar Paciente</t>
+  </si>
+  <si>
+    <t>Registrar el traspaso de un determinado paciente de un alumno a otro</t>
+  </si>
+  <si>
+    <t>Responsable de aceptar la suscripcion de un alumno a una materia/catedra determinada, (autorizar las atenciones).</t>
+  </si>
+  <si>
+    <t>Visualiza datos estadisticos e informes generados por el sistema</t>
   </si>
 </sst>
 </file>
@@ -601,7 +607,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -617,6 +623,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -685,7 +703,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -727,10 +745,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1027,8 +1057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1044,7 +1074,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>1</v>
@@ -1055,7 +1085,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -1157,7 +1187,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>19</v>
@@ -1169,10 +1199,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30">
@@ -1268,12 +1298,12 @@
         <v>34</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30">
       <c r="A20" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B20" s="4">
         <v>19</v>
@@ -1335,16 +1365,16 @@
     </row>
     <row r="25" spans="1:4" ht="30">
       <c r="A25" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="B25" s="15">
+        <v>177</v>
+      </c>
+      <c r="B25" s="16">
         <v>24</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="D25" s="18" t="s">
         <v>186</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30">
@@ -1353,10 +1383,10 @@
         <v>25</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="45">
@@ -1365,10 +1395,10 @@
         <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1377,10 +1407,10 @@
         <v>27</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30">
@@ -1389,10 +1419,10 @@
         <v>28</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="30">
@@ -1401,25 +1431,23 @@
         <v>29</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="30">
       <c r="A31" s="13"/>
-      <c r="B31" s="4">
-        <v>30</v>
-      </c>
+      <c r="B31" s="4"/>
       <c r="C31" s="2" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="30">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="45">
       <c r="A32" s="13"/>
       <c r="B32" s="4">
         <v>31</v>
@@ -1428,7 +1456,7 @@
         <v>45</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="30">
@@ -1440,7 +1468,7 @@
         <v>46</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="30">
@@ -1452,7 +1480,7 @@
         <v>47</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30">
@@ -1464,12 +1492,12 @@
         <v>48</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="45">
       <c r="A36" s="12" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B36" s="4">
         <v>35</v>
@@ -1478,7 +1506,7 @@
         <v>49</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="30">
@@ -1487,10 +1515,10 @@
         <v>36</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1623,10 +1651,10 @@
         <v>47</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="30">
@@ -1635,10 +1663,10 @@
         <v>48</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="30">
@@ -1647,10 +1675,10 @@
         <v>49</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="30">
@@ -1659,10 +1687,10 @@
         <v>50</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1681,15 +1709,9 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="13"/>
-      <c r="B53" s="4">
-        <v>52</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="B53" s="4"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="3"/>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="13"/>
@@ -1697,10 +1719,10 @@
         <v>53</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1709,24 +1731,24 @@
         <v>54</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="30">
       <c r="A56" s="12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B56" s="4">
         <v>55</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="30">
@@ -1735,10 +1757,10 @@
         <v>56</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="30">
@@ -1747,76 +1769,83 @@
         <v>57</v>
       </c>
       <c r="C58" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="30">
+      <c r="A59" s="15" t="s">
         <v>149</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="30">
-      <c r="A59" s="12" t="s">
-        <v>151</v>
       </c>
       <c r="B59" s="4">
         <v>58</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="13"/>
+      <c r="A60" s="15"/>
       <c r="B60" s="4">
         <v>59</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="13"/>
+      <c r="A61" s="15"/>
       <c r="B61" s="4">
         <v>60</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="14"/>
+      <c r="A62" s="15"/>
       <c r="B62" s="4">
         <v>61</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="C63" s="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="30">
+      <c r="A63" s="15"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>184</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="A41:A51"/>
     <mergeCell ref="A52:A55"/>
     <mergeCell ref="A56:A58"/>
-    <mergeCell ref="A59:A62"/>
     <mergeCell ref="A2:A19"/>
     <mergeCell ref="A20:A24"/>
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="A38:A40"/>
     <mergeCell ref="A25:A35"/>
+    <mergeCell ref="A59:A63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -1827,8 +1856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1839,71 +1868,75 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30">
       <c r="A2" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="60">
       <c r="A3" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="45">
       <c r="A4" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30">
+      <c r="A5" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="20" t="s">
         <v>89</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="30">
-      <c r="A5" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="45">
       <c r="A6" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="45">
+      <c r="A7" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B7" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="45">
+      <c r="A8" s="19" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:2" ht="45">
-      <c r="A8" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="B8" s="20" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="30">
       <c r="A9" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="B9" s="3"/>
+        <v>133</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>191</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1928,145 +1961,145 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="45">
       <c r="A2" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30">
       <c r="A3" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="60">
       <c r="A4" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="75">
       <c r="A5" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="60">
       <c r="A6" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="60">
       <c r="A7" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="45">
       <c r="A8" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="60">
       <c r="A9" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="60">
       <c r="A10" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="60">
       <c r="A12" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="105">
       <c r="A13" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>132</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agregaron nuevas descripciones de algunos actores
</commit_message>
<xml_diff>
--- a/repository/S.A.P.O/Producto/Iteraciones/Iteracion_01/02_Documento_Requerimiento/Funcionalidad por Paquetes.xlsx
+++ b/repository/S.A.P.O/Producto/Iteraciones/Iteracion_01/02_Documento_Requerimiento/Funcionalidad por Paquetes.xlsx
@@ -270,9 +270,6 @@
     <t>Usuario</t>
   </si>
   <si>
-    <t>Responsable de gestionar el inicio y fin de la sesión, y cambiar la contraseña.</t>
-  </si>
-  <si>
     <t>Administrador de Sistema</t>
   </si>
   <si>
@@ -285,9 +282,6 @@
     <t>Alumno</t>
   </si>
   <si>
-    <t>Responsable de realizar las atenciones a cada uno los pacientes (completar)</t>
-  </si>
-  <si>
     <t>Paciente</t>
   </si>
   <si>
@@ -555,9 +549,6 @@
     <t>Modificar los datos basicos de un Paciente en el sistema</t>
   </si>
   <si>
-    <t>Responsable de cargar los datos básicos de un paciente cuando se presenta en Recepción para ser atendido.</t>
-  </si>
-  <si>
     <t>Se encarga de realizar las tareas automáticas del sistema, como anulaciones o generacion de Historias Clinicas.</t>
   </si>
   <si>
@@ -592,6 +583,15 @@
   </si>
   <si>
     <t>Visualiza datos estadisticos e informes generados por el sistema</t>
+  </si>
+  <si>
+    <t>Cualquier persona con permiso de acceso al sistema</t>
+  </si>
+  <si>
+    <t>Puede asignarse pacientes para atenderlos y registrar el resultado de las atenciones que realiza.</t>
+  </si>
+  <si>
+    <t>Encargado de cargar los datos de un paciente y realizarle un diagnóstico cuando el mismo se presenta para solicitar ser atendido.</t>
   </si>
 </sst>
 </file>
@@ -703,7 +703,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -736,6 +736,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -747,19 +757,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1074,7 +1071,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>1</v>
@@ -1084,8 +1081,8 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="12" t="s">
-        <v>157</v>
+      <c r="A2" s="16" t="s">
+        <v>155</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -1098,7 +1095,7 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="13"/>
+      <c r="A3" s="17"/>
       <c r="B3" s="4">
         <v>2</v>
       </c>
@@ -1110,7 +1107,7 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="13"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="4">
         <v>3</v>
       </c>
@@ -1122,7 +1119,7 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="13"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="4">
         <v>4</v>
       </c>
@@ -1134,7 +1131,7 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="13"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="4">
         <v>5</v>
       </c>
@@ -1146,7 +1143,7 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="13"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="4">
         <v>6</v>
       </c>
@@ -1158,7 +1155,7 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="13"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="4">
         <v>7</v>
       </c>
@@ -1170,7 +1167,7 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="13"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="4">
         <v>8</v>
       </c>
@@ -1182,31 +1179,31 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="13"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="4">
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="13"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="4">
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30">
-      <c r="A12" s="13"/>
+      <c r="A12" s="17"/>
       <c r="B12" s="4">
         <v>11</v>
       </c>
@@ -1218,7 +1215,7 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="13"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="4">
         <v>12</v>
       </c>
@@ -1230,7 +1227,7 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="13"/>
+      <c r="A14" s="17"/>
       <c r="B14" s="4">
         <v>13</v>
       </c>
@@ -1242,7 +1239,7 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="13"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="4">
         <v>14</v>
       </c>
@@ -1254,7 +1251,7 @@
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="13"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="4">
         <v>15</v>
       </c>
@@ -1266,7 +1263,7 @@
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="13"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="4">
         <v>16</v>
       </c>
@@ -1278,7 +1275,7 @@
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="13"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="4">
         <v>17</v>
       </c>
@@ -1290,7 +1287,7 @@
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="14"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="4">
         <v>18</v>
       </c>
@@ -1298,12 +1295,12 @@
         <v>34</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30">
-      <c r="A20" s="12" t="s">
-        <v>162</v>
+      <c r="A20" s="16" t="s">
+        <v>160</v>
       </c>
       <c r="B20" s="4">
         <v>19</v>
@@ -1316,7 +1313,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="30">
-      <c r="A21" s="13"/>
+      <c r="A21" s="17"/>
       <c r="B21" s="4">
         <v>20</v>
       </c>
@@ -1328,7 +1325,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="30">
-      <c r="A22" s="13"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="4">
         <v>21</v>
       </c>
@@ -1340,7 +1337,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="30">
-      <c r="A23" s="13"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="4">
         <v>22</v>
       </c>
@@ -1352,7 +1349,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="30">
-      <c r="A24" s="14"/>
+      <c r="A24" s="18"/>
       <c r="B24" s="4">
         <v>23</v>
       </c>
@@ -1364,91 +1361,91 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="30">
-      <c r="A25" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="B25" s="16">
+      <c r="A25" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="B25" s="12">
         <v>24</v>
       </c>
-      <c r="C25" s="17" t="s">
-        <v>185</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>186</v>
+      <c r="C25" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30">
-      <c r="A26" s="13"/>
+      <c r="A26" s="17"/>
       <c r="B26" s="4">
         <v>25</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="45">
-      <c r="A27" s="13"/>
+      <c r="A27" s="17"/>
       <c r="B27" s="4">
         <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="13"/>
+      <c r="A28" s="17"/>
       <c r="B28" s="4">
         <v>27</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30">
-      <c r="A29" s="13"/>
+      <c r="A29" s="17"/>
       <c r="B29" s="4">
         <v>28</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="30">
-      <c r="A30" s="13"/>
+      <c r="A30" s="17"/>
       <c r="B30" s="4">
         <v>29</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="30">
-      <c r="A31" s="13"/>
+      <c r="A31" s="17"/>
       <c r="B31" s="4"/>
       <c r="C31" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="45">
-      <c r="A32" s="13"/>
+      <c r="A32" s="17"/>
       <c r="B32" s="4">
         <v>31</v>
       </c>
@@ -1456,11 +1453,11 @@
         <v>45</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="30">
-      <c r="A33" s="13"/>
+      <c r="A33" s="17"/>
       <c r="B33" s="4">
         <v>32</v>
       </c>
@@ -1468,11 +1465,11 @@
         <v>46</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="30">
-      <c r="A34" s="13"/>
+      <c r="A34" s="17"/>
       <c r="B34" s="4">
         <v>33</v>
       </c>
@@ -1480,11 +1477,11 @@
         <v>47</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30">
-      <c r="A35" s="14"/>
+      <c r="A35" s="18"/>
       <c r="B35" s="4">
         <v>34</v>
       </c>
@@ -1492,12 +1489,12 @@
         <v>48</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="45">
-      <c r="A36" s="12" t="s">
-        <v>173</v>
+      <c r="A36" s="16" t="s">
+        <v>171</v>
       </c>
       <c r="B36" s="4">
         <v>35</v>
@@ -1506,23 +1503,23 @@
         <v>49</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="30">
-      <c r="A37" s="14"/>
+      <c r="A37" s="18"/>
       <c r="B37" s="4">
         <v>36</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="16" t="s">
         <v>50</v>
       </c>
       <c r="B38" s="4">
@@ -1536,7 +1533,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="30">
-      <c r="A39" s="13"/>
+      <c r="A39" s="17"/>
       <c r="B39" s="4">
         <v>38</v>
       </c>
@@ -1548,7 +1545,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="30">
-      <c r="A40" s="14"/>
+      <c r="A40" s="18"/>
       <c r="B40" s="4">
         <v>39</v>
       </c>
@@ -1560,7 +1557,7 @@
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="16" t="s">
         <v>57</v>
       </c>
       <c r="B41" s="4">
@@ -1574,7 +1571,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="30">
-      <c r="A42" s="13"/>
+      <c r="A42" s="17"/>
       <c r="B42" s="4">
         <v>41</v>
       </c>
@@ -1586,7 +1583,7 @@
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="13"/>
+      <c r="A43" s="17"/>
       <c r="B43" s="4">
         <v>42</v>
       </c>
@@ -1598,7 +1595,7 @@
       </c>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="13"/>
+      <c r="A44" s="17"/>
       <c r="B44" s="4">
         <v>43</v>
       </c>
@@ -1610,7 +1607,7 @@
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="13"/>
+      <c r="A45" s="17"/>
       <c r="B45" s="4">
         <v>44</v>
       </c>
@@ -1622,7 +1619,7 @@
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="13"/>
+      <c r="A46" s="17"/>
       <c r="B46" s="4">
         <v>45</v>
       </c>
@@ -1634,7 +1631,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="30">
-      <c r="A47" s="13"/>
+      <c r="A47" s="17"/>
       <c r="B47" s="4">
         <v>46</v>
       </c>
@@ -1646,55 +1643,55 @@
       </c>
     </row>
     <row r="48" spans="1:4" ht="30">
-      <c r="A48" s="13"/>
+      <c r="A48" s="17"/>
       <c r="B48" s="4">
         <v>47</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="30">
-      <c r="A49" s="13"/>
+      <c r="A49" s="17"/>
       <c r="B49" s="4">
         <v>48</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="30">
-      <c r="A50" s="13"/>
+      <c r="A50" s="17"/>
       <c r="B50" s="4">
         <v>49</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="30">
-      <c r="A51" s="14"/>
+      <c r="A51" s="18"/>
       <c r="B51" s="4">
         <v>50</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="12" t="s">
+      <c r="A52" s="16" t="s">
         <v>72</v>
       </c>
       <c r="B52" s="4">
@@ -1708,13 +1705,13 @@
       </c>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="13"/>
+      <c r="A53" s="17"/>
       <c r="B53" s="4"/>
       <c r="C53" s="2"/>
       <c r="D53" s="3"/>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="13"/>
+      <c r="A54" s="17"/>
       <c r="B54" s="4">
         <v>53</v>
       </c>
@@ -1726,7 +1723,7 @@
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="14"/>
+      <c r="A55" s="18"/>
       <c r="B55" s="4">
         <v>54</v>
       </c>
@@ -1738,83 +1735,83 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="30">
-      <c r="A56" s="12" t="s">
-        <v>142</v>
+      <c r="A56" s="16" t="s">
+        <v>140</v>
       </c>
       <c r="B56" s="4">
         <v>55</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="30">
-      <c r="A57" s="13"/>
+      <c r="A57" s="17"/>
       <c r="B57" s="4">
         <v>56</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="30">
-      <c r="A58" s="14"/>
+      <c r="A58" s="18"/>
       <c r="B58" s="4">
         <v>57</v>
       </c>
       <c r="C58" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="30">
+      <c r="A59" s="19" t="s">
         <v>147</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="30">
-      <c r="A59" s="15" t="s">
-        <v>149</v>
       </c>
       <c r="B59" s="4">
         <v>58</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="15"/>
+      <c r="A60" s="19"/>
       <c r="B60" s="4">
         <v>59</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="15"/>
+      <c r="A61" s="19"/>
       <c r="B61" s="4">
         <v>60</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="15"/>
+      <c r="A62" s="19"/>
       <c r="B62" s="4">
         <v>61</v>
       </c>
@@ -1826,17 +1823,18 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30">
-      <c r="A63" s="15"/>
+      <c r="A63" s="19"/>
       <c r="B63" s="2"/>
       <c r="C63" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A59:A63"/>
     <mergeCell ref="A41:A51"/>
     <mergeCell ref="A52:A55"/>
     <mergeCell ref="A56:A58"/>
@@ -1845,7 +1843,6 @@
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="A38:A40"/>
     <mergeCell ref="A25:A35"/>
-    <mergeCell ref="A59:A63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -1857,7 +1854,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1879,63 +1876,63 @@
         <v>83</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>84</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="60">
       <c r="A3" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="45">
       <c r="A4" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="45">
+      <c r="A5" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="30">
-      <c r="A5" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>89</v>
+      <c r="B5" s="3" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="45">
       <c r="A6" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="45">
       <c r="A7" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="45">
-      <c r="A8" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>179</v>
+      <c r="A8" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30">
       <c r="A9" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -1961,145 +1958,145 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="45">
       <c r="A2" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30">
       <c r="A3" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="60">
       <c r="A4" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="75">
       <c r="A5" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="60">
       <c r="A6" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="60">
       <c r="A7" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="45">
       <c r="A8" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="60">
       <c r="A9" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="60">
       <c r="A10" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="60">
       <c r="A12" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="105">
       <c r="A13" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>130</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se modificó  el documento Funcionalidad por Paquetes.xlsx y el documento Modelos UML Iteracion_01.eap
</commit_message>
<xml_diff>
--- a/repository/S.A.P.O/Producto/Iteraciones/Iteracion_01/02_Documento_Requerimiento/Funcionalidad por Paquetes.xlsx
+++ b/repository/S.A.P.O/Producto/Iteraciones/Iteracion_01/02_Documento_Requerimiento/Funcionalidad por Paquetes.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Funcionalidad por Paquete" sheetId="1" r:id="rId1"/>
     <sheet name="Actores" sheetId="3" r:id="rId2"/>
-    <sheet name="RNF" sheetId="4" r:id="rId3"/>
+    <sheet name="Especificación de RNF" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="176">
   <si>
     <t>Paquete</t>
   </si>
@@ -294,123 +294,12 @@
     <t>Responsable de Recepcion de Pacientes</t>
   </si>
   <si>
-    <t>Numero</t>
-  </si>
-  <si>
-    <t>Requerimientos No Funcionales</t>
-  </si>
-  <si>
-    <t>Descripción</t>
-  </si>
-  <si>
-    <t>1.</t>
-  </si>
-  <si>
     <t>Entorno web</t>
   </si>
   <si>
     <t>Se requiere entorno web para la gestión de solicitudes de inscripción, consulta del estado del trámite o cancelación del mismo y reserva de recursos</t>
   </si>
   <si>
-    <t>2.</t>
-  </si>
-  <si>
-    <t>Formato de solicitud de inscripción</t>
-  </si>
-  <si>
-    <t>Se imprimirá en hoja A4 con el membrete y una marca de agua de la SeCyT</t>
-  </si>
-  <si>
-    <t>3.</t>
-  </si>
-  <si>
-    <t>Clave de usuario</t>
-  </si>
-  <si>
-    <t>Debe ser alfanumérica de entre 6 y 12 caracteres UNICODE, con las siguientes restricciones: al menos 2 caracteres deben ser letras, no se permite una secuencia de letras o números mayor a tres elementos.</t>
-  </si>
-  <si>
-    <t>4.</t>
-  </si>
-  <si>
-    <t>Reportes de información</t>
-  </si>
-  <si>
-    <t>Deberán tener el membrete de la SeCyT (uso del logo en el encabezado) Identificación del reporte mediante el título establecido en el encabezado, en letra Times New Roman, centrado, con fuente 16 y numeración de las páginas del reporte.</t>
-  </si>
-  <si>
-    <t>5.</t>
-  </si>
-  <si>
-    <t>Distinción de disponibilidad de recursos</t>
-  </si>
-  <si>
-    <t>El científico solicitante podrá distinguir rápido y fácilmente los días en los cuales el recurso no está disponible, mediante el uso de colores, de los días en los que aún se puede registrar una reserva.</t>
-  </si>
-  <si>
-    <t>6.</t>
-  </si>
-  <si>
-    <t>Soporte del sistema (a usuarios)</t>
-  </si>
-  <si>
-    <t>El sistema se deberá desarrollar para soportar una carga de usuarios conectados en forma simultánea de aproximadamente 100. La cantidad de transacciones por segundo a resolver no ascendería las 250</t>
-  </si>
-  <si>
-    <t>7.</t>
-  </si>
-  <si>
-    <t>Interfaz gráfica</t>
-  </si>
-  <si>
-    <t>Todas las pantallas del sistema deberán contar con el logo de la SeCyT en el extremo superior izquierdo y se utilizarán colores acordes con dicha imagen</t>
-  </si>
-  <si>
-    <t>8.</t>
-  </si>
-  <si>
-    <t>Base de Datos y copias de respaldo</t>
-  </si>
-  <si>
-    <t>La base de datos deberá estar fragmentada para lograr una mayor disponibilidad. Se estableció la realización de copias de restauración periódicas para lograr la recuperación ante fallas. Dichas copias se realizarán en discos RAID 1</t>
-  </si>
-  <si>
-    <t>9.</t>
-  </si>
-  <si>
-    <t>Navegadores</t>
-  </si>
-  <si>
-    <t>Los navegadores que deberán soportar la aplicación son las versiones Google Chrome 4, Internet Explorer 8, Mozilla FireFox 3.2, Opera 10 y superiores. La aplicación también será accesible desde dispositivos móviles.</t>
-  </si>
-  <si>
-    <t>10.</t>
-  </si>
-  <si>
-    <t>Aplicaciones</t>
-  </si>
-  <si>
-    <t>La aplicación será multiplataforma</t>
-  </si>
-  <si>
-    <t>11.</t>
-  </si>
-  <si>
-    <t>Seguridad</t>
-  </si>
-  <si>
-    <t>El sistema limitará el número de intentos de conexión no exitosos a 3, momento a partir del cual se inhabilita el usuario y se rechazan otros intentos hasta la correspondiente autorización del usuario supervisor.</t>
-  </si>
-  <si>
-    <t>12.</t>
-  </si>
-  <si>
-    <t>Almacenamiento digital</t>
-  </si>
-  <si>
-    <t>La SeCyT pretende que el sistema tienda a minimizar el uso del papel mediante la generación y uso de la mayor cantidad de archivos y documentos electrónicos e imágenes digitales. También solicitó que los documentos presentados al momento de presentar la Solicitud de Inscripción  del Centro de Investigación sean digitalizados mediante algún dispositivo.</t>
-  </si>
-  <si>
     <t>Autoridad</t>
   </si>
   <si>
@@ -592,13 +481,76 @@
   </si>
   <si>
     <t>Encargado de cargar los datos de un paciente y realizarle un diagnóstico cuando el mismo se presenta para solicitar ser atendido.</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>NOMBRE</t>
+  </si>
+  <si>
+    <t>DESCRIPCION</t>
+  </si>
+  <si>
+    <t>TIPO</t>
+  </si>
+  <si>
+    <t>AFECTA A LA ARQUITECTURA</t>
+  </si>
+  <si>
+    <t>JUSTIFICACIÓN</t>
+  </si>
+  <si>
+    <t>PRIORIDAD</t>
+  </si>
+  <si>
+    <t>Organizacional - Implementación</t>
+  </si>
+  <si>
+    <t>Plazo de entrega</t>
+  </si>
+  <si>
+    <t>El 80% del sistema debe estar finalizado para fines de noviembre de 2013</t>
+  </si>
+  <si>
+    <t>Organizacional - Entrega</t>
+  </si>
+  <si>
+    <t>Privacidad de las Historias Clinicas</t>
+  </si>
+  <si>
+    <t>El sistema solo revelará información básica acerca de las historias clinicas de los pacientes  debido a los datos sensibles de las mismas.</t>
+  </si>
+  <si>
+    <t>Externos - Legislativos - Privacidad</t>
+  </si>
+  <si>
+    <t>Permisos Usuarios</t>
+  </si>
+  <si>
+    <t>El sistema deberá implementar distintos privilegios para sus usuarios, a fin de que cierta información solo sea accesible para los usuarios con permisos sobre ella.</t>
+  </si>
+  <si>
+    <t>La implementación del sistema no debe interferir con el normal funcionamiento de los servicios del servidor de la facultad.</t>
+  </si>
+  <si>
+    <t>Independecia de los sistemas actuales</t>
+  </si>
+  <si>
+    <t>Rendimiento</t>
+  </si>
+  <si>
+    <t>El registro de usuario, carga de datos, registro y consulta de paciente deben responder con eficiencia.</t>
+  </si>
+  <si>
+    <t>Producto - Eficiencia - Desempeño</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -703,7 +655,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -727,12 +679,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -746,6 +692,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -756,7 +705,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -764,6 +725,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -810,7 +779,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -842,9 +811,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -876,6 +846,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1051,14 +1022,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
@@ -1066,12 +1037,12 @@
     <col min="4" max="4" width="43.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>154</v>
+        <v>117</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>1</v>
@@ -1080,9 +1051,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="16" t="s">
-        <v>155</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>118</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -1094,8 +1065,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="17"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
       <c r="B3" s="4">
         <v>2</v>
       </c>
@@ -1106,8 +1077,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="17"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
       <c r="B4" s="4">
         <v>3</v>
       </c>
@@ -1118,8 +1089,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="17"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
       <c r="B5" s="4">
         <v>4</v>
       </c>
@@ -1130,8 +1101,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="17"/>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
       <c r="B6" s="4">
         <v>5</v>
       </c>
@@ -1142,8 +1113,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="17"/>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
       <c r="B7" s="4">
         <v>6</v>
       </c>
@@ -1154,8 +1125,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="17"/>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
       <c r="B8" s="4">
         <v>7</v>
       </c>
@@ -1166,8 +1137,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="17"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
       <c r="B9" s="4">
         <v>8</v>
       </c>
@@ -1178,32 +1149,32 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="17"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
       <c r="B10" s="4">
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>156</v>
+        <v>119</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="17"/>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
       <c r="B11" s="4">
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>157</v>
+        <v>120</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30">
-      <c r="A12" s="17"/>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
       <c r="B12" s="4">
         <v>11</v>
       </c>
@@ -1214,8 +1185,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="17"/>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
       <c r="B13" s="4">
         <v>12</v>
       </c>
@@ -1226,8 +1197,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="17"/>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
       <c r="B14" s="4">
         <v>13</v>
       </c>
@@ -1238,8 +1209,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="17"/>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
       <c r="B15" s="4">
         <v>14</v>
       </c>
@@ -1250,8 +1221,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="17"/>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
       <c r="B16" s="4">
         <v>15</v>
       </c>
@@ -1262,8 +1233,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="17"/>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="16"/>
       <c r="B17" s="4">
         <v>16</v>
       </c>
@@ -1274,8 +1245,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="17"/>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="16"/>
       <c r="B18" s="4">
         <v>17</v>
       </c>
@@ -1286,8 +1257,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="18"/>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="17"/>
       <c r="B19" s="4">
         <v>18</v>
       </c>
@@ -1295,12 +1266,12 @@
         <v>34</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="30">
-      <c r="A20" s="16" t="s">
-        <v>160</v>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>123</v>
       </c>
       <c r="B20" s="4">
         <v>19</v>
@@ -1312,8 +1283,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30">
-      <c r="A21" s="17"/>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="16"/>
       <c r="B21" s="4">
         <v>20</v>
       </c>
@@ -1324,8 +1295,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30">
-      <c r="A22" s="17"/>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
       <c r="B22" s="4">
         <v>21</v>
       </c>
@@ -1336,8 +1307,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30">
-      <c r="A23" s="17"/>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="16"/>
       <c r="B23" s="4">
         <v>22</v>
       </c>
@@ -1348,8 +1319,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30">
-      <c r="A24" s="18"/>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
       <c r="B24" s="4">
         <v>23</v>
       </c>
@@ -1360,92 +1331,92 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30">
-      <c r="A25" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="B25" s="12">
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" s="10">
         <v>24</v>
       </c>
-      <c r="C25" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="30">
-      <c r="A26" s="17"/>
+      <c r="C25" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="16"/>
       <c r="B26" s="4">
         <v>25</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>161</v>
+        <v>124</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="45">
-      <c r="A27" s="17"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="16"/>
       <c r="B27" s="4">
         <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>163</v>
+        <v>126</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="17"/>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="16"/>
       <c r="B28" s="4">
         <v>27</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>165</v>
+        <v>128</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="30">
-      <c r="A29" s="17"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="16"/>
       <c r="B29" s="4">
         <v>28</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>167</v>
+        <v>130</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="30">
-      <c r="A30" s="17"/>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="16"/>
       <c r="B30" s="4">
         <v>29</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>169</v>
+        <v>132</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="30">
-      <c r="A31" s="17"/>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="16"/>
       <c r="B31" s="4"/>
       <c r="C31" s="2" t="s">
-        <v>185</v>
+        <v>148</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="45">
-      <c r="A32" s="17"/>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="16"/>
       <c r="B32" s="4">
         <v>31</v>
       </c>
@@ -1453,11 +1424,11 @@
         <v>45</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="30">
-      <c r="A33" s="17"/>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="16"/>
       <c r="B33" s="4">
         <v>32</v>
       </c>
@@ -1465,11 +1436,11 @@
         <v>46</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="30">
-      <c r="A34" s="17"/>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="16"/>
       <c r="B34" s="4">
         <v>33</v>
       </c>
@@ -1477,11 +1448,11 @@
         <v>47</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="30">
-      <c r="A35" s="18"/>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="17"/>
       <c r="B35" s="4">
         <v>34</v>
       </c>
@@ -1489,12 +1460,12 @@
         <v>48</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="45">
-      <c r="A36" s="16" t="s">
-        <v>171</v>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
+        <v>134</v>
       </c>
       <c r="B36" s="4">
         <v>35</v>
@@ -1503,23 +1474,23 @@
         <v>49</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="30">
-      <c r="A37" s="18"/>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="17"/>
       <c r="B37" s="4">
         <v>36</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>173</v>
+        <v>136</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="15" t="s">
         <v>50</v>
       </c>
       <c r="B38" s="4">
@@ -1532,8 +1503,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30">
-      <c r="A39" s="17"/>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="16"/>
       <c r="B39" s="4">
         <v>38</v>
       </c>
@@ -1544,8 +1515,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30">
-      <c r="A40" s="18"/>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="17"/>
       <c r="B40" s="4">
         <v>39</v>
       </c>
@@ -1556,8 +1527,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="16" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="15" t="s">
         <v>57</v>
       </c>
       <c r="B41" s="4">
@@ -1570,8 +1541,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="30">
-      <c r="A42" s="17"/>
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="16"/>
       <c r="B42" s="4">
         <v>41</v>
       </c>
@@ -1582,8 +1553,8 @@
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="17"/>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="16"/>
       <c r="B43" s="4">
         <v>42</v>
       </c>
@@ -1594,8 +1565,8 @@
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="17"/>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="16"/>
       <c r="B44" s="4">
         <v>43</v>
       </c>
@@ -1606,8 +1577,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="17"/>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="16"/>
       <c r="B45" s="4">
         <v>44</v>
       </c>
@@ -1618,8 +1589,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="17"/>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="16"/>
       <c r="B46" s="4">
         <v>45</v>
       </c>
@@ -1630,8 +1601,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="30">
-      <c r="A47" s="17"/>
+    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="16"/>
       <c r="B47" s="4">
         <v>46</v>
       </c>
@@ -1642,56 +1613,56 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="30">
-      <c r="A48" s="17"/>
+    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="16"/>
       <c r="B48" s="4">
         <v>47</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>132</v>
+        <v>95</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="30">
-      <c r="A49" s="17"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="16"/>
       <c r="B49" s="4">
         <v>48</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>134</v>
+        <v>97</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="30">
-      <c r="A50" s="17"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="16"/>
       <c r="B50" s="4">
         <v>49</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>136</v>
+        <v>99</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="30">
-      <c r="A51" s="18"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="17"/>
       <c r="B51" s="4">
         <v>50</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>138</v>
+        <v>101</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="15" t="s">
         <v>72</v>
       </c>
       <c r="B52" s="4">
@@ -1704,14 +1675,14 @@
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="17"/>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="16"/>
       <c r="B53" s="4"/>
       <c r="C53" s="2"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="17"/>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="16"/>
       <c r="B54" s="4">
         <v>53</v>
       </c>
@@ -1722,8 +1693,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="18"/>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="17"/>
       <c r="B55" s="4">
         <v>54</v>
       </c>
@@ -1734,84 +1705,84 @@
         <v>78</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="30">
-      <c r="A56" s="16" t="s">
-        <v>140</v>
+    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="15" t="s">
+        <v>103</v>
       </c>
       <c r="B56" s="4">
         <v>55</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>141</v>
+        <v>104</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="30">
-      <c r="A57" s="17"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="16"/>
       <c r="B57" s="4">
         <v>56</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>143</v>
+        <v>106</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="30">
-      <c r="A58" s="18"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="17"/>
       <c r="B58" s="4">
         <v>57</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>145</v>
+        <v>108</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="30">
-      <c r="A59" s="19" t="s">
-        <v>147</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="14" t="s">
+        <v>110</v>
       </c>
       <c r="B59" s="4">
         <v>58</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>148</v>
+        <v>111</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="19"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="14"/>
       <c r="B60" s="4">
         <v>59</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>150</v>
+        <v>113</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="19"/>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="14"/>
       <c r="B61" s="4">
         <v>60</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>152</v>
+        <v>115</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="19"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="14"/>
       <c r="B62" s="4">
         <v>61</v>
       </c>
@@ -1822,14 +1793,14 @@
         <v>80</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="30">
-      <c r="A63" s="19"/>
+    <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="14"/>
       <c r="B63" s="2"/>
       <c r="C63" s="3" t="s">
-        <v>180</v>
+        <v>143</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>181</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1850,20 +1821,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>81</v>
       </c>
@@ -1871,15 +1842,15 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30">
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>83</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="60">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>84</v>
       </c>
@@ -1887,23 +1858,23 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="45">
+    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>86</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="45">
-      <c r="A5" s="15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
         <v>87</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="45">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>88</v>
       </c>
@@ -1911,28 +1882,28 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="45">
+    <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>90</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="45">
-      <c r="A8" s="15" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
         <v>91</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="30">
-      <c r="A9" s="11" t="s">
-        <v>131</v>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>94</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1942,164 +1913,283 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="18">
+        <v>1</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C2" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="45">
-      <c r="A2" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="30">
-      <c r="A3" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="60">
-      <c r="A4" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="75">
-      <c r="A5" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>105</v>
+      <c r="D2" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="18">
+        <v>2</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+    </row>
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="18">
+        <v>3</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+    </row>
+    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="18">
+        <v>4</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>169</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="60">
-      <c r="A6" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="60">
-      <c r="A7" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="45">
-      <c r="A8" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="60">
-      <c r="A9" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="60">
-      <c r="A10" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="60">
-      <c r="A12" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="105">
-      <c r="A13" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>130</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+    </row>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="18">
+        <v>5</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+    </row>
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="18">
+        <v>6</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="18">
+        <v>7</v>
+      </c>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="18">
+        <v>8</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="18">
+        <v>9</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="18">
+        <v>10</v>
+      </c>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="18">
+        <v>11</v>
+      </c>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="18">
+        <v>12</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="18">
+        <v>13</v>
+      </c>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="18">
+        <v>14</v>
+      </c>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="18">
+        <v>15</v>
+      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="18">
+        <v>16</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="18">
+        <v>18</v>
+      </c>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>